<commit_message>
Modified @AfterClass, Used Assertions, Created BaseClass and Added Comments.
</commit_message>
<xml_diff>
--- a/Automation_Framework/resources/testdata.xlsx
+++ b/Automation_Framework/resources/testdata.xlsx
@@ -7,23 +7,16 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="19980" windowHeight="8070"/>
   </bookViews>
   <sheets>
-    <sheet name="credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="productinfo" sheetId="3" r:id="rId2"/>
-    <sheet name="deliveryaddress" sheetId="4" r:id="rId3"/>
-    <sheet name="payment" sheetId="5" r:id="rId4"/>
+    <sheet name="productinfo" sheetId="3" r:id="rId1"/>
+    <sheet name="deliveryaddress" sheetId="4" r:id="rId2"/>
+    <sheet name="payment" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>productname</t>
   </si>
@@ -34,13 +27,7 @@
     <t>productdescription</t>
   </si>
   <si>
-    <t>https://www.flipkart.com/</t>
-  </si>
-  <si>
     <t>camera</t>
-  </si>
-  <si>
-    <t>url</t>
   </si>
   <si>
     <t>searchproduct</t>
@@ -104,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,14 +103,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,16 +140,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -184,8 +160,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,51 +460,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -543,21 +476,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -569,72 +502,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
-    <col min="4" max="4" width="18.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="18.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -642,7 +575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -658,34 +591,34 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5">
         <v>2020</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>26</v>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ExtentReporting Implemented along with the listeners. Removed Complicated Driver Initialization code also as per the feedback received.
</commit_message>
<xml_diff>
--- a/Automation_Framework/resources/testdata.xlsx
+++ b/Automation_Framework/resources/testdata.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="19980" windowHeight="8070"/>
   </bookViews>
   <sheets>
-    <sheet name="productinfo" sheetId="3" r:id="rId1"/>
-    <sheet name="deliveryaddress" sheetId="4" r:id="rId2"/>
-    <sheet name="payment" sheetId="5" r:id="rId3"/>
+    <sheet name="productinfo" sheetId="4" r:id="rId1"/>
+    <sheet name="address" sheetId="5" r:id="rId2"/>
+    <sheet name="paymenttype" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>productname</t>
   </si>
@@ -85,6 +85,27 @@
   </si>
   <si>
     <t>000</t>
+  </si>
+  <si>
+    <t>dharam</t>
+  </si>
+  <si>
+    <t>Ramamurthy Nagar</t>
+  </si>
+  <si>
+    <t>Harikrishna Layout</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Dooravani Medical</t>
+  </si>
+  <si>
+    <t>Home</t>
   </si>
 </sst>
 </file>
@@ -143,14 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -463,13 +481,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -498,7 +516,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -506,23 +523,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="18.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -558,20 +570,37 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7338214702</v>
+      </c>
+      <c r="C2" s="4">
+        <v>560016</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -580,13 +609,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,22 +639,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2020</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning of the Code from the Test Class and shifted to the particular Page classes. Now Test class holds only the business scenarios related invokations.
</commit_message>
<xml_diff>
--- a/Automation_Framework/resources/testdata.xlsx
+++ b/Automation_Framework/resources/testdata.xlsx
@@ -4,28 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="19980" windowHeight="8070"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="14220" windowHeight="6675" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="productinfo" sheetId="4" r:id="rId1"/>
     <sheet name="address" sheetId="5" r:id="rId2"/>
     <sheet name="paymenttype" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>productname</t>
-  </si>
-  <si>
-    <t>productprice</t>
-  </si>
-  <si>
-    <t>productdescription</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>camera</t>
   </si>
@@ -480,39 +472,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -539,39 +516,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4">
         <v>7338214702</v>
@@ -580,23 +557,23 @@
         <v>560016</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -608,49 +585,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4">
         <v>2020</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testdata.xlsx Updated with the raw data.
</commit_message>
<xml_diff>
--- a/Automation_Framework/resources/testdata.xlsx
+++ b/Automation_Framework/resources/testdata.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="14220" windowHeight="6675" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="14220" windowHeight="6675" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="productinfo" sheetId="4" r:id="rId1"/>
-    <sheet name="address" sheetId="5" r:id="rId2"/>
+    <sheet name="deliveryaddress" sheetId="5" r:id="rId2"/>
     <sheet name="paymenttype" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>camera</t>
   </si>
@@ -98,6 +97,21 @@
   </si>
   <si>
     <t>Home</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>productprice</t>
+  </si>
+  <si>
+    <t>productdescription</t>
+  </si>
+  <si>
+    <t>7338214702</t>
+  </si>
+  <si>
+    <t>560016</t>
   </si>
 </sst>
 </file>
@@ -473,23 +487,38 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -500,7 +529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -550,11 +581,11 @@
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4">
-        <v>7338214702</v>
-      </c>
-      <c r="C2" s="4">
-        <v>560016</v>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>21</v>
@@ -578,6 +609,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -585,7 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>